<commit_message>
Preprocessing of timeseries data done
</commit_message>
<xml_diff>
--- a/results/Results_pvfactors.xlsx
+++ b/results/Results_pvfactors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21140" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Software Info" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="99">
   <si>
     <t>Name of Software</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>All three: DNI, DHI and GHI</t>
-  </si>
-  <si>
-    <t>The sun position is provided as input to the model and is not calculated</t>
   </si>
   <si>
     <t>Yes</t>
@@ -1014,7 +1011,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1253,6 +1250,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1572,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1724,8 +1722,8 @@
       <c r="B22" t="s">
         <v>29</v>
       </c>
-      <c r="C22" t="s">
-        <v>90</v>
+      <c r="C22" s="94">
+        <v>0.47916666666666669</v>
       </c>
     </row>
     <row r="24" spans="2:3">
@@ -1738,7 +1736,7 @@
         <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="2:3">
@@ -1746,7 +1744,7 @@
         <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="2:3">
@@ -1754,7 +1752,7 @@
         <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="2:3">
@@ -1762,7 +1760,7 @@
         <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="2:3">
@@ -1770,7 +1768,7 @@
         <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="2:3">
@@ -1783,7 +1781,7 @@
         <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="2:3">
@@ -1791,7 +1789,7 @@
         <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="2:3">
@@ -1799,7 +1797,7 @@
         <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="2:3">
@@ -1807,7 +1805,7 @@
         <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="2:3">
@@ -1815,7 +1813,7 @@
         <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="2:3">
@@ -1823,7 +1821,7 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1841,8 +1839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AI39"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1931,9 +1929,7 @@
       <c r="J6" s="80"/>
       <c r="K6" s="80"/>
       <c r="L6" s="81"/>
-      <c r="P6" s="56" t="s">
-        <v>37</v>
-      </c>
+      <c r="P6" s="56"/>
       <c r="Q6" s="57"/>
       <c r="R6" s="57"/>
       <c r="S6" s="57"/>
@@ -2990,7 +2986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AI39"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:G7"/>
     </sheetView>
   </sheetViews>
@@ -4138,7 +4134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AI39"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:G7"/>
     </sheetView>
   </sheetViews>
@@ -5286,8 +5282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AI39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:G7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Now have end to end simulation steps
</commit_message>
<xml_diff>
--- a/results/Results_pvfactors.xlsx
+++ b/results/Results_pvfactors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21140" activeTab="4"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="Software Info" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="100">
   <si>
     <t>Name of Software</t>
   </si>
@@ -312,9 +312,6 @@
     <t>Marc Abou Anoma</t>
   </si>
   <si>
-    <t>regular laptop (CPU-based simulations), in my case macOS</t>
-  </si>
-  <si>
     <t>2D VF</t>
   </si>
   <si>
@@ -372,6 +369,12 @@
   </si>
   <si>
     <t>No, the software assumes infinitely long PV rows (because of the 2D geometry) and does not account for edge effects</t>
+  </si>
+  <si>
+    <t>30s</t>
+  </si>
+  <si>
+    <t>regular laptop (CPU-based simulations), in my case MacBook Pro 2013</t>
   </si>
 </sst>
 </file>
@@ -1570,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1617,7 +1620,7 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="2:3">
@@ -1625,7 +1628,7 @@
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:3">
@@ -1633,7 +1636,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="140">
@@ -1641,7 +1644,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="93" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="140">
@@ -1649,7 +1652,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="93" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="2:3">
@@ -1657,7 +1660,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="92" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="2:3">
@@ -1670,7 +1673,7 @@
         <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="2:3">
@@ -1678,7 +1681,7 @@
         <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="2:3">
@@ -1686,7 +1689,7 @@
         <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="2:3">
@@ -1694,7 +1697,7 @@
         <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="2:3">
@@ -1707,7 +1710,7 @@
         <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="2:3">
@@ -1715,7 +1718,7 @@
         <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="2:3">
@@ -1736,7 +1739,7 @@
         <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="2:3">
@@ -1744,7 +1747,7 @@
         <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="2:3">
@@ -1752,7 +1755,7 @@
         <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="2:3">
@@ -1760,7 +1763,7 @@
         <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="2:3">
@@ -1768,7 +1771,7 @@
         <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="2:3">
@@ -1781,7 +1784,7 @@
         <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="2:3">
@@ -1789,7 +1792,7 @@
         <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="2:3">
@@ -1797,7 +1800,7 @@
         <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="2:3">
@@ -1805,7 +1808,7 @@
         <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="2:3">
@@ -1813,7 +1816,7 @@
         <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="2:3">
@@ -1821,7 +1824,7 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1839,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AI39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2054,7 +2057,9 @@
       <c r="C11" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="15"/>
+      <c r="D11" s="15" t="s">
+        <v>98</v>
+      </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -2088,7 +2093,9 @@
       <c r="C12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="16"/>
+      <c r="D12" s="16" t="s">
+        <v>98</v>
+      </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -2122,7 +2129,9 @@
       <c r="C13" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="17"/>
+      <c r="D13" s="17" t="s">
+        <v>98</v>
+      </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -5282,7 +5291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AI39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>

</xml_diff>